<commit_message>
fix results output issue
</commit_message>
<xml_diff>
--- a/Model_Results/Result_global.xlsx
+++ b/Model_Results/Result_global.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,25 +468,48 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>SVM_global</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>84.02777777777779</v>
+        <v>86.22448979591836</v>
       </c>
       <c r="C2" t="n">
-        <v>91.66666666666666</v>
+        <v>92.85714285714286</v>
       </c>
       <c r="D2" t="n">
-        <v>91.66666666666666</v>
+        <v>92.85714285714286</v>
       </c>
       <c r="E2" t="n">
-        <v>87.68115942028986</v>
+        <v>89.41798941798943</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5600448933782267</v>
+        <v>0.3153210425937699</v>
       </c>
       <c r="G2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>AdaBoostClassifier_global</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>86.09271523178806</v>
+      </c>
+      <c r="C3" t="n">
+        <v>90.90909090909091</v>
+      </c>
+      <c r="D3" t="n">
+        <v>90.90909090909091</v>
+      </c>
+      <c r="E3" t="n">
+        <v>88.43537414965988</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.659249841068023</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added fix in preprocessing and machine learning codes
</commit_message>
<xml_diff>
--- a/Model_Results/Result_global.xlsx
+++ b/Model_Results/Result_global.xlsx
@@ -436,17 +436,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>precision</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>recall</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>92.85714285714286</v>
+      </c>
+      <c r="C2" t="n">
         <v>86.22448979591836</v>
-      </c>
-      <c r="C2" t="n">
-        <v>92.85714285714286</v>
       </c>
       <c r="D2" t="n">
         <v>92.85714285714286</v>
@@ -495,19 +495,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>86.09271523178806</v>
+        <v>90.25974025974025</v>
       </c>
       <c r="C3" t="n">
-        <v>90.90909090909091</v>
+        <v>86.04761904761904</v>
       </c>
       <c r="D3" t="n">
-        <v>90.90909090909091</v>
+        <v>90.25974025974025</v>
       </c>
       <c r="E3" t="n">
-        <v>88.43537414965988</v>
+        <v>88.10336421257922</v>
       </c>
       <c r="F3" t="n">
-        <v>0.659249841068023</v>
+        <v>0.6223776223776223</v>
       </c>
       <c r="G3" t="inlineStr"/>
     </row>

</xml_diff>